<commit_message>
save some data in StateSpace.xlsx
</commit_message>
<xml_diff>
--- a/experiments/StateSpace.xlsx
+++ b/experiments/StateSpace.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amber\Documents\UvA\Master Jaar 2\Minor Programmeren\Programmeertheorie\Proteins\Proteins\experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marrit\Documents\School\2017-2018\Heuristieken\Proteins\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28685DE-FBE2-450B-A87F-0028967BBA71}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF7D757-19FF-4E85-9F4A-E2AF507D0AA6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
   <si>
     <t>Randomizer</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t xml:space="preserve">bij 77520000 keer prunen op -9 … </t>
+  </si>
+  <si>
+    <t>bij 2660000 iteraties en 1090000 keer prunen -19</t>
   </si>
 </sst>
 </file>
@@ -1120,24 +1123,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" topLeftCell="G3" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="26.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="25.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.19921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="3.5" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="18.75" customWidth="1"/>
-    <col min="8" max="8" width="18.75" style="5" customWidth="1"/>
-    <col min="9" max="23" width="10.75" customWidth="1"/>
-    <col min="24" max="27" width="25.75" customWidth="1"/>
-    <col min="28" max="28" width="20.75" customWidth="1"/>
+    <col min="7" max="7" width="18.69921875" customWidth="1"/>
+    <col min="8" max="8" width="18.69921875" style="5" customWidth="1"/>
+    <col min="9" max="23" width="10.69921875" customWidth="1"/>
+    <col min="24" max="27" width="25.69921875" customWidth="1"/>
+    <col min="28" max="28" width="20.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="40.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="40.200000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="54" t="s">
         <v>12</v>
       </c>
@@ -1188,7 +1191,7 @@
       <c r="V1" s="49"/>
       <c r="W1" s="51"/>
     </row>
-    <row r="2" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="55"/>
       <c r="B2" s="57"/>
       <c r="C2" s="59"/>
@@ -1243,7 +1246,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="25.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1320,7 +1323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>1</v>
       </c>
@@ -1389,7 +1392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>2</v>
       </c>
@@ -1466,7 +1469,7 @@
         <v>2.7954578399658203E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>2</v>
       </c>
@@ -1535,7 +1538,7 @@
         <v>2.8696484240489538E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>3</v>
       </c>
@@ -1612,7 +1615,7 @@
         <v>8.9785316959023476E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>3</v>
       </c>
@@ -1675,7 +1678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>4</v>
       </c>
@@ -1748,7 +1751,7 @@
         <v>1.3552527156068805E-17</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>4</v>
       </c>
@@ -1809,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>5</v>
       </c>
@@ -1878,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>5</v>
       </c>
@@ -1939,7 +1942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>6</v>
       </c>
@@ -2006,7 +2009,7 @@
         <v>1.6263032587282567E-17</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>6</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>7</v>
       </c>
@@ -2117,14 +2120,16 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U15" s="19"/>
+      <c r="U15" s="19" t="s">
+        <v>25</v>
+      </c>
       <c r="V15" s="18"/>
       <c r="W15" s="42">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>7</v>
       </c>
@@ -2179,7 +2184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>8</v>
       </c>
@@ -2242,7 +2247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>8</v>
       </c>
@@ -2297,7 +2302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>9</v>
       </c>
@@ -2360,7 +2365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13">
         <v>9</v>
       </c>
@@ -2415,7 +2420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="25.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" ht="25.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G21" s="1"/>
       <c r="H21" s="4"/>
       <c r="I21" s="1"/>
@@ -2429,7 +2434,7 @@
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
     </row>
-    <row r="22" spans="1:23" ht="25.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" ht="25.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I22" s="28"/>
       <c r="J22" t="s">
         <v>18</v>
@@ -2441,7 +2446,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="25.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="I23" s="27"/>
       <c r="J23" t="s">
         <v>19</v>
@@ -2451,18 +2456,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I24" s="29"/>
       <c r="J24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:23" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="49">
     <mergeCell ref="B7:B8"/>

</xml_diff>